<commit_message>
First attempt at matrix schedule
</commit_message>
<xml_diff>
--- a/test/mechanical/forecasts/ReportWeek4.xlsx
+++ b/test/mechanical/forecasts/ReportWeek4.xlsx
@@ -14,9 +14,9 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="28">
-  <si>
-    <t>City</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="29">
+  <si>
+    <t>Location</t>
   </si>
   <si>
     <t>Quality</t>
@@ -98,6 +98,9 @@
   </si>
   <si>
     <t>Glendale</t>
+  </si>
+  <si>
+    <t>SF</t>
   </si>
 </sst>
 </file>
@@ -110,7 +113,7 @@
     <numFmt numFmtId="166" formatCode="#0%"/>
     <numFmt numFmtId="167" formatCode="#0"/>
   </numFmts>
-  <fonts count="4">
+  <fonts count="5">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -137,13 +140,21 @@
     <font>
       <b/>
       <sz val="11"/>
+      <color rgb="FFE6BE8A"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -159,6 +170,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FF003B48"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFAF1E2C"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -190,7 +207,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -198,7 +215,10 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
@@ -507,7 +527,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C26"/>
+  <dimension ref="A1:F26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
@@ -519,289 +539,443 @@
     <col min="1" max="1" width="20.7109375" customWidth="1"/>
     <col min="2" max="3" width="8.28515625" customWidth="1"/>
     <col min="4" max="4" width="1.7109375" customWidth="1"/>
+    <col min="5" max="6" width="8.28515625" customWidth="1"/>
+    <col min="7" max="7" width="1.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:6">
       <c r="B1" s="1" t="s">
         <v>25</v>
       </c>
       <c r="C1" s="2" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="2" spans="1:3">
-      <c r="A2" s="3" t="s">
+      <c r="E1" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6">
+      <c r="A2" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="4" t="s">
-        <v>27</v>
-      </c>
-      <c r="C2" s="4"/>
-    </row>
-    <row r="3" spans="1:3">
-      <c r="A3" s="3" t="s">
+      <c r="B2" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2" s="5"/>
+      <c r="E2" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="F2" s="5"/>
+    </row>
+    <row r="3" spans="1:6">
+      <c r="A3" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="5">
-        <v>0.641028762672984</v>
-      </c>
-      <c r="C3" s="5"/>
-    </row>
-    <row r="4" spans="1:3">
-      <c r="A4" s="3" t="s">
+      <c r="B3" s="6">
+        <v>0.645183171759773</v>
+      </c>
+      <c r="C3" s="6"/>
+      <c r="E3" s="6">
+        <v>0.8368484051341047</v>
+      </c>
+      <c r="F3" s="6"/>
+    </row>
+    <row r="4" spans="1:6">
+      <c r="A4" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="5">
-        <v>0.4453927573491729</v>
-      </c>
-      <c r="C4" s="5"/>
-    </row>
-    <row r="5" spans="1:3">
-      <c r="A5" s="3" t="s">
+      <c r="B4" s="6">
+        <v>0.09997087051259206</v>
+      </c>
+      <c r="C4" s="6"/>
+      <c r="E4" s="6">
+        <v>0.9988048236851483</v>
+      </c>
+      <c r="F4" s="6"/>
+    </row>
+    <row r="5" spans="1:6">
+      <c r="A5" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B5" s="4">
-        <v>28.55095681470489</v>
-      </c>
-      <c r="C5" s="4"/>
-    </row>
-    <row r="6" spans="1:3">
-      <c r="A6" s="3" t="s">
+      <c r="B5" s="5">
+        <v>6.449952332089971</v>
+      </c>
+      <c r="C5" s="5"/>
+      <c r="E5" s="5">
+        <v>83.58482237411671</v>
+      </c>
+      <c r="F5" s="5"/>
+    </row>
+    <row r="6" spans="1:6">
+      <c r="A6" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="B6" s="6">
-        <v>0.9073078</v>
-      </c>
-      <c r="C6" s="6">
-        <v>0.0926922</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3">
-      <c r="A7" s="3" t="s">
+      <c r="B6" s="7">
+        <v>0.9870177999999999</v>
+      </c>
+      <c r="C6" s="7">
+        <v>0.0129822</v>
+      </c>
+      <c r="E6" s="7">
+        <v>0.4796505</v>
+      </c>
+      <c r="F6" s="7">
+        <v>0.5203495</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6">
+      <c r="A7" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="B7" s="7">
-        <v>32.3945594</v>
-      </c>
-      <c r="C7" s="7">
-        <v>20.3044472</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3">
-      <c r="A8" s="3" t="s">
+      <c r="B7" s="8">
+        <v>33.7943326</v>
+      </c>
+      <c r="C7" s="8">
+        <v>16.1711158</v>
+      </c>
+      <c r="E7" s="8">
+        <v>24.0370666</v>
+      </c>
+      <c r="F7" s="8">
+        <v>24.8267312</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6">
+      <c r="A8" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="B8" s="7">
-        <v>20</v>
-      </c>
-      <c r="C8" s="7">
+      <c r="B8" s="8">
+        <v>23</v>
+      </c>
+      <c r="C8" s="8">
         <v>9</v>
       </c>
-    </row>
-    <row r="9" spans="1:3">
-      <c r="A9" s="3" t="s">
+      <c r="E8" s="8">
+        <v>13</v>
+      </c>
+      <c r="F8" s="8">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6">
+      <c r="A9" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="B9" s="7">
+      <c r="B9" s="8">
+        <v>26</v>
+      </c>
+      <c r="C9" s="8">
+        <v>10</v>
+      </c>
+      <c r="E9" s="8">
+        <v>17</v>
+      </c>
+      <c r="F9" s="8">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6">
+      <c r="A10" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="B10" s="8">
+        <v>27</v>
+      </c>
+      <c r="C10" s="8">
+        <v>12</v>
+      </c>
+      <c r="E10" s="8">
+        <v>18</v>
+      </c>
+      <c r="F10" s="8">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6">
+      <c r="A11" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="B11" s="8">
+        <v>28</v>
+      </c>
+      <c r="C11" s="8">
+        <v>13</v>
+      </c>
+      <c r="E11" s="8">
+        <v>20</v>
+      </c>
+      <c r="F11" s="8">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6">
+      <c r="A12" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="B12" s="8">
+        <v>31</v>
+      </c>
+      <c r="C12" s="8">
+        <v>13</v>
+      </c>
+      <c r="E12" s="8">
+        <v>20</v>
+      </c>
+      <c r="F12" s="8">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6">
+      <c r="A13" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="B13" s="8">
+        <v>31</v>
+      </c>
+      <c r="C13" s="8">
+        <v>13</v>
+      </c>
+      <c r="E13" s="8">
+        <v>20</v>
+      </c>
+      <c r="F13" s="8">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6">
+      <c r="A14" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="B14" s="8">
+        <v>33</v>
+      </c>
+      <c r="C14" s="8">
+        <v>16</v>
+      </c>
+      <c r="E14" s="8">
+        <v>21</v>
+      </c>
+      <c r="F14" s="8">
         <v>24</v>
       </c>
-      <c r="C9" s="7">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3">
-      <c r="A10" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="B10" s="7">
+    </row>
+    <row r="15" spans="1:6">
+      <c r="A15" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="B15" s="8">
+        <v>33</v>
+      </c>
+      <c r="C15" s="8">
+        <v>16</v>
+      </c>
+      <c r="E15" s="8">
+        <v>24</v>
+      </c>
+      <c r="F15" s="8">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6">
+      <c r="A16" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="B16" s="8">
+        <v>34</v>
+      </c>
+      <c r="C16" s="8">
+        <v>17</v>
+      </c>
+      <c r="E16" s="8">
+        <v>24</v>
+      </c>
+      <c r="F16" s="8">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6">
+      <c r="A17" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="B17" s="8">
+        <v>34</v>
+      </c>
+      <c r="C17" s="8">
+        <v>17</v>
+      </c>
+      <c r="E17" s="8">
+        <v>25</v>
+      </c>
+      <c r="F17" s="8">
         <v>26</v>
       </c>
-      <c r="C10" s="7">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3">
-      <c r="A11" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="B11" s="7">
-        <v>27</v>
-      </c>
-      <c r="C11" s="7">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3">
-      <c r="A12" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="B12" s="7">
+    </row>
+    <row r="18" spans="1:6">
+      <c r="A18" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="B18" s="8">
+        <v>34</v>
+      </c>
+      <c r="C18" s="8">
+        <v>17</v>
+      </c>
+      <c r="E18" s="8">
+        <v>27</v>
+      </c>
+      <c r="F18" s="8">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6">
+      <c r="A19" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="B19" s="8">
+        <v>35</v>
+      </c>
+      <c r="C19" s="8">
+        <v>19</v>
+      </c>
+      <c r="E19" s="8">
+        <v>27</v>
+      </c>
+      <c r="F19" s="8">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6">
+      <c r="A20" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="B20" s="8">
+        <v>37</v>
+      </c>
+      <c r="C20" s="8">
+        <v>19</v>
+      </c>
+      <c r="E20" s="8">
+        <v>27</v>
+      </c>
+      <c r="F20" s="8">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6">
+      <c r="A21" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="B21" s="8">
+        <v>38</v>
+      </c>
+      <c r="C21" s="8">
+        <v>20</v>
+      </c>
+      <c r="E21" s="8">
+        <v>27</v>
+      </c>
+      <c r="F21" s="8">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6">
+      <c r="A22" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="B22" s="8">
+        <v>39</v>
+      </c>
+      <c r="C22" s="8">
+        <v>20</v>
+      </c>
+      <c r="E22" s="8">
+        <v>27</v>
+      </c>
+      <c r="F22" s="8">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6">
+      <c r="A23" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="B23" s="8">
+        <v>40</v>
+      </c>
+      <c r="C23" s="8">
+        <v>20</v>
+      </c>
+      <c r="E23" s="8">
         <v>28</v>
       </c>
-      <c r="C12" s="7">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3">
-      <c r="A13" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="B13" s="7">
-        <v>30</v>
-      </c>
-      <c r="C13" s="7">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3">
-      <c r="A14" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="B14" s="7">
+      <c r="F23" s="8">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6">
+      <c r="A24" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="B24" s="8">
+        <v>41</v>
+      </c>
+      <c r="C24" s="8">
+        <v>20</v>
+      </c>
+      <c r="E24" s="8">
+        <v>28</v>
+      </c>
+      <c r="F24" s="8">
         <v>31</v>
       </c>
-      <c r="C14" s="7">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3">
-      <c r="A15" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="B15" s="7">
-        <v>31</v>
-      </c>
-      <c r="C15" s="7">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3">
-      <c r="A16" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="B16" s="7">
-        <v>32</v>
-      </c>
-      <c r="C16" s="7">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3">
-      <c r="A17" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="B17" s="7">
+    </row>
+    <row r="25" spans="1:6">
+      <c r="A25" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="B25" s="8">
+        <v>41</v>
+      </c>
+      <c r="C25" s="8">
+        <v>20</v>
+      </c>
+      <c r="E25" s="8">
         <v>33</v>
       </c>
-      <c r="C17" s="7">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3">
-      <c r="A18" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="B18" s="7">
+      <c r="F25" s="8">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6">
+      <c r="A26" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="B26" s="8">
+        <v>42</v>
+      </c>
+      <c r="C26" s="8">
+        <v>20</v>
+      </c>
+      <c r="E26" s="8">
         <v>34</v>
       </c>
-      <c r="C18" s="7">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3">
-      <c r="A19" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="B19" s="7">
+      <c r="F26" s="8">
         <v>34</v>
       </c>
-      <c r="C19" s="7">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3">
-      <c r="A20" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="B20" s="7">
-        <v>35</v>
-      </c>
-      <c r="C20" s="7">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3">
-      <c r="A21" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="B21" s="7">
-        <v>37</v>
-      </c>
-      <c r="C21" s="7">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3">
-      <c r="A22" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="B22" s="7">
-        <v>38</v>
-      </c>
-      <c r="C22" s="7">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3">
-      <c r="A23" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="B23" s="7">
-        <v>38</v>
-      </c>
-      <c r="C23" s="7">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="24" spans="1:3">
-      <c r="A24" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="B24" s="7">
-        <v>40</v>
-      </c>
-      <c r="C24" s="7">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="25" spans="1:3">
-      <c r="A25" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="B25" s="7">
-        <v>41</v>
-      </c>
-      <c r="C25" s="7">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="26" spans="1:3">
-      <c r="A26" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="B26" s="7">
-        <v>41</v>
-      </c>
-      <c r="C26" s="7">
-        <v>30</v>
-      </c>
     </row>
   </sheetData>
-  <mergeCells count="4">
+  <mergeCells count="8">
     <mergeCell ref="B2:C2"/>
     <mergeCell ref="B3:C3"/>
     <mergeCell ref="B4:C4"/>
     <mergeCell ref="B5:C5"/>
+    <mergeCell ref="E2:F2"/>
+    <mergeCell ref="E3:F3"/>
+    <mergeCell ref="E4:F4"/>
+    <mergeCell ref="E5:F5"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Added validity check for score tables
</commit_message>
<xml_diff>
--- a/test/mechanical/forecasts/ReportWeek4.xlsx
+++ b/test/mechanical/forecasts/ReportWeek4.xlsx
@@ -575,11 +575,11 @@
         <v>1</v>
       </c>
       <c r="B3" s="6">
-        <v>0.645183171759773</v>
+        <v>0.6459373893103791</v>
       </c>
       <c r="C3" s="6"/>
       <c r="E3" s="6">
-        <v>0.8368484051341047</v>
+        <v>0.8380898705323252</v>
       </c>
       <c r="F3" s="6"/>
     </row>
@@ -588,11 +588,11 @@
         <v>2</v>
       </c>
       <c r="B4" s="6">
-        <v>0.09997087051259206</v>
+        <v>0.09960389109914584</v>
       </c>
       <c r="C4" s="6"/>
       <c r="E4" s="6">
-        <v>0.9988048236851483</v>
+        <v>0.9987932693766906</v>
       </c>
       <c r="F4" s="6"/>
     </row>
@@ -601,11 +601,11 @@
         <v>3</v>
       </c>
       <c r="B5" s="5">
-        <v>6.449952332089971</v>
+        <v>6.433787738173758</v>
       </c>
       <c r="C5" s="5"/>
       <c r="E5" s="5">
-        <v>83.58482237411671</v>
+        <v>83.70785218204684</v>
       </c>
       <c r="F5" s="5"/>
     </row>
@@ -614,16 +614,16 @@
         <v>4</v>
       </c>
       <c r="B6" s="7">
-        <v>0.9870177999999999</v>
+        <v>0.9870765</v>
       </c>
       <c r="C6" s="7">
-        <v>0.0129822</v>
+        <v>0.0129235</v>
       </c>
       <c r="E6" s="7">
-        <v>0.4796505</v>
+        <v>0.4795524</v>
       </c>
       <c r="F6" s="7">
-        <v>0.5203495</v>
+        <v>0.5204476</v>
       </c>
     </row>
     <row r="7" spans="1:6">
@@ -631,16 +631,16 @@
         <v>5</v>
       </c>
       <c r="B7" s="8">
-        <v>33.7943326</v>
+        <v>33.7868016</v>
       </c>
       <c r="C7" s="8">
-        <v>16.1711158</v>
+        <v>16.1652718</v>
       </c>
       <c r="E7" s="8">
-        <v>24.0370666</v>
+        <v>24.0421396</v>
       </c>
       <c r="F7" s="8">
-        <v>24.8267312</v>
+        <v>24.8297674</v>
       </c>
     </row>
     <row r="8" spans="1:6">

</xml_diff>